<commit_message>
Add summation and verify total net paayment
</commit_message>
<xml_diff>
--- a/Data Files/Test Data.xlsx
+++ b/Data Files/Test Data.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aditia\git\hre_test\Data Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3C3A2F5B-404C-440B-841C-24CA7793B379}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64287C2C-A591-4708-B8D1-991218CA9474}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{24326381-8BEC-45D3-BC51-8ABD6EF7D704}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="25">
   <si>
     <t>Name</t>
   </si>
@@ -105,6 +106,12 @@
   </si>
   <si>
     <t>Test Employee 11</t>
+  </si>
+  <si>
+    <t>Curr</t>
+  </si>
+  <si>
+    <t>SGD</t>
   </si>
 </sst>
 </file>
@@ -485,10 +492,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{391E7384-A072-4B6F-A8B1-C9FE83A7EF78}">
-  <dimension ref="A1:H12"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="I12" sqref="A4:I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -502,7 +509,7 @@
     <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -527,8 +534,11 @@
       <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I1" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -553,8 +563,11 @@
       <c r="H2">
         <v>4003</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -579,8 +592,122 @@
       <c r="H3">
         <v>4859.75</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96FBF4EA-5FD4-4CA3-AADB-8DD58EB52034}">
+  <dimension ref="A1:I12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2">
+        <v>4000</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2">
+        <v>7</v>
+      </c>
+      <c r="F2">
+        <v>10</v>
+      </c>
+      <c r="G2">
+        <v>3993</v>
+      </c>
+      <c r="H2">
+        <v>4003</v>
+      </c>
+      <c r="I2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3">
+        <v>5000</v>
+      </c>
+      <c r="C3">
+        <v>1850</v>
+      </c>
+      <c r="D3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3">
+        <v>1.5</v>
+      </c>
+      <c r="F3">
+        <v>11.25</v>
+      </c>
+      <c r="G3">
+        <v>3998.5</v>
+      </c>
+      <c r="H3">
+        <v>4859.75</v>
+      </c>
+      <c r="I3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -602,8 +729,11 @@
       <c r="H4">
         <v>6011.25</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -628,8 +758,11 @@
       <c r="H5">
         <v>6779.25</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>15</v>
       </c>
@@ -654,8 +787,11 @@
       <c r="H6">
         <v>7755.25</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>17</v>
       </c>
@@ -680,8 +816,11 @@
       <c r="H7">
         <v>8999.25</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>18</v>
       </c>
@@ -706,8 +845,11 @@
       <c r="H8">
         <v>9786.25</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I8" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>19</v>
       </c>
@@ -729,8 +871,11 @@
       <c r="H9">
         <v>11011.25</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I9" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>20</v>
       </c>
@@ -755,8 +900,11 @@
       <c r="H10">
         <v>11763.25</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I10" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>21</v>
       </c>
@@ -781,8 +929,11 @@
       <c r="H11">
         <v>12745.25</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I11" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>22</v>
       </c>
@@ -806,6 +957,9 @@
       </c>
       <c r="H12">
         <v>13993.25</v>
+      </c>
+      <c r="I12" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Enhance draft while loop, add formatter, add release payroll
</commit_message>
<xml_diff>
--- a/Data Files/Test Data.xlsx
+++ b/Data Files/Test Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aditia\git\hre_test\Data Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64287C2C-A591-4708-B8D1-991218CA9474}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{414C56EA-54F6-4A44-9A0F-C9E9E3735EC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{24326381-8BEC-45D3-BC51-8ABD6EF7D704}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="25">
   <si>
     <t>Name</t>
   </si>
@@ -492,10 +492,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{391E7384-A072-4B6F-A8B1-C9FE83A7EF78}">
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I12" sqref="A4:I12"/>
+      <selection activeCell="A5" sqref="A5:I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -596,6 +596,261 @@
         <v>24</v>
       </c>
     </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4">
+        <v>6000</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>11.25</v>
+      </c>
+      <c r="G4">
+        <v>6000</v>
+      </c>
+      <c r="H4">
+        <v>6011.25</v>
+      </c>
+      <c r="I4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5">
+        <v>7000</v>
+      </c>
+      <c r="C5">
+        <v>2590</v>
+      </c>
+      <c r="D5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5">
+        <v>22</v>
+      </c>
+      <c r="F5">
+        <v>11.25</v>
+      </c>
+      <c r="G5">
+        <v>5578</v>
+      </c>
+      <c r="H5">
+        <v>6779.25</v>
+      </c>
+      <c r="I5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6">
+        <v>8000</v>
+      </c>
+      <c r="C6">
+        <v>2738</v>
+      </c>
+      <c r="D6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6">
+        <v>34</v>
+      </c>
+      <c r="F6">
+        <v>11.25</v>
+      </c>
+      <c r="G6">
+        <v>6486</v>
+      </c>
+      <c r="H6">
+        <v>7755.25</v>
+      </c>
+      <c r="I6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7">
+        <v>9000</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7">
+        <v>12</v>
+      </c>
+      <c r="F7">
+        <v>11.25</v>
+      </c>
+      <c r="G7">
+        <v>8988</v>
+      </c>
+      <c r="H7">
+        <v>8999.25</v>
+      </c>
+      <c r="I7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8">
+        <v>10000</v>
+      </c>
+      <c r="C8">
+        <v>2738</v>
+      </c>
+      <c r="D8" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8">
+        <v>3</v>
+      </c>
+      <c r="F8">
+        <v>11.25</v>
+      </c>
+      <c r="G8">
+        <v>8517</v>
+      </c>
+      <c r="H8">
+        <v>9786.25</v>
+      </c>
+      <c r="I8" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9">
+        <v>11000</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <v>11.25</v>
+      </c>
+      <c r="G9">
+        <v>11000</v>
+      </c>
+      <c r="H9">
+        <v>11011.25</v>
+      </c>
+      <c r="I9" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10">
+        <v>12000</v>
+      </c>
+      <c r="C10">
+        <v>2738</v>
+      </c>
+      <c r="D10" t="s">
+        <v>14</v>
+      </c>
+      <c r="E10">
+        <v>26</v>
+      </c>
+      <c r="F10">
+        <v>11.25</v>
+      </c>
+      <c r="G10">
+        <v>10494</v>
+      </c>
+      <c r="H10">
+        <v>11763.25</v>
+      </c>
+      <c r="I10" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11">
+        <v>13000</v>
+      </c>
+      <c r="C11">
+        <v>2738</v>
+      </c>
+      <c r="D11" t="s">
+        <v>16</v>
+      </c>
+      <c r="E11">
+        <v>44</v>
+      </c>
+      <c r="F11">
+        <v>11.25</v>
+      </c>
+      <c r="G11">
+        <v>11476</v>
+      </c>
+      <c r="H11">
+        <v>12745.25</v>
+      </c>
+      <c r="I11" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12">
+        <v>14000</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E12">
+        <v>18</v>
+      </c>
+      <c r="F12">
+        <v>11.25</v>
+      </c>
+      <c r="G12">
+        <v>13982</v>
+      </c>
+      <c r="H12">
+        <v>13993.25</v>
+      </c>
+      <c r="I12" t="s">
+        <v>24</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -606,7 +861,7 @@
   <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="A5" sqref="A5:I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Add single iteration scenario and step def, add logout
</commit_message>
<xml_diff>
--- a/Data Files/Test Data.xlsx
+++ b/Data Files/Test Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aditia\git\hre_test\Data Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{414C56EA-54F6-4A44-9A0F-C9E9E3735EC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2C6C602-5A07-437E-A8D4-7C1ADCE73AB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{24326381-8BEC-45D3-BC51-8ABD6EF7D704}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{24326381-8BEC-45D3-BC51-8ABD6EF7D704}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="25">
   <si>
     <t>Name</t>
   </si>
@@ -492,10 +492,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{391E7384-A072-4B6F-A8B1-C9FE83A7EF78}">
-  <dimension ref="A1:I12"/>
+  <dimension ref="A1:I6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:I12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -680,177 +680,6 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>17</v>
-      </c>
-      <c r="B7">
-        <v>9000</v>
-      </c>
-      <c r="C7">
-        <v>0</v>
-      </c>
-      <c r="D7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E7">
-        <v>12</v>
-      </c>
-      <c r="F7">
-        <v>11.25</v>
-      </c>
-      <c r="G7">
-        <v>8988</v>
-      </c>
-      <c r="H7">
-        <v>8999.25</v>
-      </c>
-      <c r="I7" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>18</v>
-      </c>
-      <c r="B8">
-        <v>10000</v>
-      </c>
-      <c r="C8">
-        <v>2738</v>
-      </c>
-      <c r="D8" t="s">
-        <v>11</v>
-      </c>
-      <c r="E8">
-        <v>3</v>
-      </c>
-      <c r="F8">
-        <v>11.25</v>
-      </c>
-      <c r="G8">
-        <v>8517</v>
-      </c>
-      <c r="H8">
-        <v>9786.25</v>
-      </c>
-      <c r="I8" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>19</v>
-      </c>
-      <c r="B9">
-        <v>11000</v>
-      </c>
-      <c r="C9">
-        <v>0</v>
-      </c>
-      <c r="E9">
-        <v>0</v>
-      </c>
-      <c r="F9">
-        <v>11.25</v>
-      </c>
-      <c r="G9">
-        <v>11000</v>
-      </c>
-      <c r="H9">
-        <v>11011.25</v>
-      </c>
-      <c r="I9" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>20</v>
-      </c>
-      <c r="B10">
-        <v>12000</v>
-      </c>
-      <c r="C10">
-        <v>2738</v>
-      </c>
-      <c r="D10" t="s">
-        <v>14</v>
-      </c>
-      <c r="E10">
-        <v>26</v>
-      </c>
-      <c r="F10">
-        <v>11.25</v>
-      </c>
-      <c r="G10">
-        <v>10494</v>
-      </c>
-      <c r="H10">
-        <v>11763.25</v>
-      </c>
-      <c r="I10" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>21</v>
-      </c>
-      <c r="B11">
-        <v>13000</v>
-      </c>
-      <c r="C11">
-        <v>2738</v>
-      </c>
-      <c r="D11" t="s">
-        <v>16</v>
-      </c>
-      <c r="E11">
-        <v>44</v>
-      </c>
-      <c r="F11">
-        <v>11.25</v>
-      </c>
-      <c r="G11">
-        <v>11476</v>
-      </c>
-      <c r="H11">
-        <v>12745.25</v>
-      </c>
-      <c r="I11" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>22</v>
-      </c>
-      <c r="B12">
-        <v>14000</v>
-      </c>
-      <c r="C12">
-        <v>0</v>
-      </c>
-      <c r="D12" t="s">
-        <v>9</v>
-      </c>
-      <c r="E12">
-        <v>18</v>
-      </c>
-      <c r="F12">
-        <v>11.25</v>
-      </c>
-      <c r="G12">
-        <v>13982</v>
-      </c>
-      <c r="H12">
-        <v>13993.25</v>
-      </c>
-      <c r="I12" t="s">
-        <v>24</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -860,8 +689,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96FBF4EA-5FD4-4CA3-AADB-8DD58EB52034}">
   <dimension ref="A1:I12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:I12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Add randomstring as a new payroll and store to data file
</commit_message>
<xml_diff>
--- a/Data Files/Test Data.xlsx
+++ b/Data Files/Test Data.xlsx
@@ -1,24 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27932"/>
   <workbookPr defaultThemeVersion="202300"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aditia\git\hre_test\Data Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2C6C602-5A07-437E-A8D4-7C1ADCE73AB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr documentId="13_ncr:1_{EAB9B313-A2B2-4143-94B2-B0A946ED41AC}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{24326381-8BEC-45D3-BC51-8ABD6EF7D704}"/>
+    <workbookView activeTab="2" windowHeight="15720" windowWidth="29040" xWindow="-120" xr2:uid="{24326381-8BEC-45D3-BC51-8ABD6EF7D704}" yWindow="-120"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet1" r:id="rId1" sheetId="1"/>
+    <sheet name="Sheet2" r:id="rId2" sheetId="2"/>
+    <sheet name="Test Name" r:id="rId3" sheetId="3"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="0"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="28">
   <si>
     <t>Name</t>
   </si>
@@ -112,12 +113,22 @@
   </si>
   <si>
     <t>SGD</t>
+  </si>
+  <si>
+    <t>Test Name</t>
+  </si>
+  <si>
+    <t>aaaaaa</t>
+  </si>
+  <si>
+    <t>uAJINIPj</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -153,17 +164,17 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -180,10 +191,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="0E2841"/>
@@ -218,7 +229,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Aptos Display" panose="02110004020202020204"/>
+        <a:latin panose="02110004020202020204" typeface="Aptos Display"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -270,7 +281,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Aptos Narrow" panose="02110004020202020204"/>
+        <a:latin panose="02110004020202020204" typeface="Aptos Narrow"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -381,21 +392,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="25400">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -412,7 +423,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -484,32 +495,32 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{2E142A2C-CD16-42D6-873A-C26D2A0506FA}" vid="{1BDDFF52-6CD6-40A5-AB3C-68EB2F1E4D0A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{2E142A2C-CD16-42D6-873A-C26D2A0506FA}" name="Office Theme" vid="{1BDDFF52-6CD6-40A5-AB3C-68EB2F1E4D0A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{391E7384-A072-4B6F-A8B1-C9FE83A7EF78}">
-  <dimension ref="A1:I6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{391E7384-A072-4B6F-A8B1-C9FE83A7EF78}">
+  <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="16.0" collapsed="false"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="11.7109375" collapsed="false"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="14.0" collapsed="false"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="22.0" collapsed="false"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="6.0" collapsed="false"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="9.85546875" collapsed="false"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="12.0" collapsed="false"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="1" s="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -622,89 +633,31 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5">
-        <v>7000</v>
-      </c>
-      <c r="C5">
-        <v>2590</v>
-      </c>
-      <c r="D5" t="s">
-        <v>14</v>
-      </c>
-      <c r="E5">
-        <v>22</v>
-      </c>
-      <c r="F5">
-        <v>11.25</v>
-      </c>
-      <c r="G5">
-        <v>5578</v>
-      </c>
-      <c r="H5">
-        <v>6779.25</v>
-      </c>
-      <c r="I5" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>15</v>
-      </c>
-      <c r="B6">
-        <v>8000</v>
-      </c>
-      <c r="C6">
-        <v>2738</v>
-      </c>
-      <c r="D6" t="s">
-        <v>16</v>
-      </c>
-      <c r="E6">
-        <v>34</v>
-      </c>
-      <c r="F6">
-        <v>11.25</v>
-      </c>
-      <c r="G6">
-        <v>6486</v>
-      </c>
-      <c r="H6">
-        <v>7755.25</v>
-      </c>
-      <c r="I6" t="s">
-        <v>24</v>
-      </c>
-    </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96FBF4EA-5FD4-4CA3-AADB-8DD58EB52034}">
-  <dimension ref="A1:I12"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96FBF4EA-5FD4-4CA3-AADB-8DD58EB52034}">
+  <dimension ref="A1:J12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="16.0" collapsed="false"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="11.7109375" collapsed="false"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="14.0" collapsed="false"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="22.0" collapsed="false"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="6.0" collapsed="false"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="9.85546875" collapsed="false"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="12.0" collapsed="false"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="1" s="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1047,6 +1000,35 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6267371-6AA0-4A44-B06D-B320EDFB1404}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" customWidth="true" width="23.7109375" collapsed="false"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup orientation="portrait" paperSize="9" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add payslip is generated for each employee on step 2
</commit_message>
<xml_diff>
--- a/Data Files/Test Data.xlsx
+++ b/Data Files/Test Data.xlsx
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="32">
   <si>
     <t>Name</t>
   </si>
@@ -122,6 +122,18 @@
   </si>
   <si>
     <t>uAJINIPj</t>
+  </si>
+  <si>
+    <t>vvGRuurG</t>
+  </si>
+  <si>
+    <t>JDXgLQLV</t>
+  </si>
+  <si>
+    <t>BYHIUDyR</t>
+  </si>
+  <si>
+    <t>nTcJqngH</t>
   </si>
 </sst>
 </file>
@@ -511,13 +523,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="16.0" collapsed="false"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="11.7109375" collapsed="false"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="14.0" collapsed="false"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="22.0" collapsed="false"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="6.0" collapsed="false"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="9.85546875" collapsed="false"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="12.0" collapsed="false"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="16.0" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="11.7109375" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="14.0" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="22.0" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="6.0" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="9.85546875" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row customFormat="1" r="1" s="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -648,13 +660,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="16.0" collapsed="false"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="11.7109375" collapsed="false"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="14.0" collapsed="false"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="22.0" collapsed="false"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="6.0" collapsed="false"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="9.85546875" collapsed="false"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="12.0" collapsed="false"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="16.0" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="11.7109375" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="14.0" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="22.0" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="6.0" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="9.85546875" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row customFormat="1" r="1" s="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -1014,7 +1026,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="23.7109375" collapsed="false"/>
+    <col min="1" max="1" customWidth="true" width="23.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
@@ -1024,7 +1036,7 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add choose record by test id, add change employee data feature and step definition, add verify total net payment after changes, add verify new payslip generated
</commit_message>
<xml_diff>
--- a/Data Files/Test Data.xlsx
+++ b/Data Files/Test Data.xlsx
@@ -1,44 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27932"/>
   <workbookPr defaultThemeVersion="202300"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aditia\git\hre_test\Data Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr documentId="13_ncr:1_{EAB9B313-A2B2-4143-94B2-B0A946ED41AC}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09B256E9-FB81-49D9-8516-EC61F0474F9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView activeTab="2" windowHeight="15720" windowWidth="29040" xWindow="-120" xr2:uid="{24326381-8BEC-45D3-BC51-8ABD6EF7D704}" yWindow="-120"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{24326381-8BEC-45D3-BC51-8ABD6EF7D704}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" r:id="rId1" sheetId="1"/>
-    <sheet name="Sheet2" r:id="rId2" sheetId="2"/>
-    <sheet name="Test Name" r:id="rId3" sheetId="3"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Test Name" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="30">
   <si>
     <t>Name</t>
   </si>
@@ -118,29 +107,22 @@
     <t>Test Name</t>
   </si>
   <si>
-    <t>aaaaaa</t>
-  </si>
-  <si>
-    <t>uAJINIPj</t>
-  </si>
-  <si>
-    <t>vvGRuurG</t>
-  </si>
-  <si>
-    <t>JDXgLQLV</t>
-  </si>
-  <si>
-    <t>BYHIUDyR</t>
-  </si>
-  <si>
-    <t>nTcJqngH</t>
+    <t>Extra Duty Allowance</t>
+  </si>
+  <si>
+    <t>Employee Name</t>
+  </si>
+  <si>
+    <t>TkmwGCjQ</t>
+  </si>
+  <si>
+    <t>100.00</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -176,17 +158,18 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0"/>
+  <cellXfs count="3">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -203,10 +186,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="0E2841"/>
@@ -241,7 +224,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin panose="02110004020202020204" typeface="Aptos Display"/>
+        <a:latin typeface="Aptos Display" panose="02110004020202020204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -293,7 +276,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin panose="02110004020202020204" typeface="Aptos Narrow"/>
+        <a:latin typeface="Aptos Narrow" panose="02110004020202020204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -404,21 +387,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="25400">
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -435,7 +418,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -507,32 +490,32 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{2E142A2C-CD16-42D6-873A-C26D2A0506FA}" name="Office Theme" vid="{1BDDFF52-6CD6-40A5-AB3C-68EB2F1E4D0A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{2E142A2C-CD16-42D6-873A-C26D2A0506FA}" vid="{1BDDFF52-6CD6-40A5-AB3C-68EB2F1E4D0A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{391E7384-A072-4B6F-A8B1-C9FE83A7EF78}">
-  <dimension ref="A1:J4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{391E7384-A072-4B6F-A8B1-C9FE83A7EF78}">
+  <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="16.0" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="11.7109375" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="14.0" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="22.0" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="6.0" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="9.85546875" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
+    <col min="1" max="1" width="16" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="14" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="22" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="6" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="9.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="12" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row customFormat="1" r="1" s="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -646,30 +629,31 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96FBF4EA-5FD4-4CA3-AADB-8DD58EB52034}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96FBF4EA-5FD4-4CA3-AADB-8DD58EB52034}">
   <dimension ref="A1:J12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="16.0" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="11.7109375" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="14.0" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="22.0" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="6.0" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="9.85546875" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
+    <col min="1" max="1" width="16" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="14" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="22" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="6" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="9.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="12" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="22" customWidth="1"/>
   </cols>
   <sheetData>
-    <row customFormat="1" r="1" s="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -697,8 +681,11 @@
       <c r="I1" s="1" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J1" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -726,8 +713,11 @@
       <c r="I2" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -755,8 +745,11 @@
       <c r="I3" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -781,8 +774,11 @@
       <c r="I4" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J4">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -810,8 +806,11 @@
       <c r="I5" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>15</v>
       </c>
@@ -839,8 +838,11 @@
       <c r="I6" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>17</v>
       </c>
@@ -868,8 +870,11 @@
       <c r="I7" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>18</v>
       </c>
@@ -897,8 +902,11 @@
       <c r="I8" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>19</v>
       </c>
@@ -923,8 +931,11 @@
       <c r="I9" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>20</v>
       </c>
@@ -952,8 +963,11 @@
       <c r="I10" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>21</v>
       </c>
@@ -981,8 +995,11 @@
       <c r="I11" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>22</v>
       </c>
@@ -1010,37 +1027,54 @@
       <c r="I12" t="s">
         <v>24</v>
       </c>
+      <c r="J12">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6267371-6AA0-4A44-B06D-B320EDFB1404}">
-  <dimension ref="A1:B2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6267371-6AA0-4A44-B06D-B320EDFB1404}">
+  <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" zoomScale="106" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="23.7109375" collapsed="true"/>
+    <col min="1" max="1" width="23.7109375" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="22.5703125" customWidth="1"/>
+    <col min="3" max="3" width="23" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>31</v>
+        <v>28</v>
+      </c>
+      <c r="B2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup orientation="portrait" paperSize="9" r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add commentation and refine verifyNetPayment method
</commit_message>
<xml_diff>
--- a/Data Files/Test Data.xlsx
+++ b/Data Files/Test Data.xlsx
@@ -1,25 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27932"/>
   <workbookPr defaultThemeVersion="202300"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aditia\git\hre_test\Data Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09B256E9-FB81-49D9-8516-EC61F0474F9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr documentId="13_ncr:1_{F7D75790-B829-498D-8C7F-686F442780FC}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{24326381-8BEC-45D3-BC51-8ABD6EF7D704}"/>
+    <workbookView windowHeight="15720" windowWidth="29040" xWindow="-120" xr2:uid="{24326381-8BEC-45D3-BC51-8ABD6EF7D704}" yWindow="-120"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Test Name" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet1" r:id="rId1" sheetId="1"/>
+    <sheet name="Sheet2" r:id="rId2" sheetId="2"/>
+    <sheet name="Test Name" r:id="rId3" sheetId="3"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="31">
   <si>
     <t>Name</t>
   </si>
@@ -113,16 +113,20 @@
     <t>Employee Name</t>
   </si>
   <si>
-    <t>TkmwGCjQ</t>
-  </si>
-  <si>
     <t>100.00</t>
+  </si>
+  <si>
+    <t>cjaUzEDo</t>
+  </si>
+  <si>
+    <t>MHArryMt</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -158,18 +162,18 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" quotePrefix="1" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -186,10 +190,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="0E2841"/>
@@ -224,7 +228,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Aptos Display" panose="02110004020202020204"/>
+        <a:latin panose="02110004020202020204" typeface="Aptos Display"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -276,7 +280,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Aptos Narrow" panose="02110004020202020204"/>
+        <a:latin panose="02110004020202020204" typeface="Aptos Narrow"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -387,21 +391,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="25400">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -418,7 +422,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -490,32 +494,32 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{2E142A2C-CD16-42D6-873A-C26D2A0506FA}" vid="{1BDDFF52-6CD6-40A5-AB3C-68EB2F1E4D0A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{2E142A2C-CD16-42D6-873A-C26D2A0506FA}" name="Office Theme" vid="{1BDDFF52-6CD6-40A5-AB3C-68EB2F1E4D0A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{391E7384-A072-4B6F-A8B1-C9FE83A7EF78}">
-  <dimension ref="A1:I4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{391E7384-A072-4B6F-A8B1-C9FE83A7EF78}">
+  <dimension ref="A1:J12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A1:I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="14" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="22" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="6" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="9.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="12" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="16.0" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="11.7109375" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="14.0" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="22.0" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="6.0" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="9.85546875" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="1" s="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -628,32 +632,261 @@
         <v>24</v>
       </c>
     </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5">
+        <v>7000</v>
+      </c>
+      <c r="C5">
+        <v>2590</v>
+      </c>
+      <c r="D5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5">
+        <v>22</v>
+      </c>
+      <c r="F5">
+        <v>11.25</v>
+      </c>
+      <c r="G5">
+        <v>5578</v>
+      </c>
+      <c r="H5">
+        <v>6779.25</v>
+      </c>
+      <c r="I5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6">
+        <v>8000</v>
+      </c>
+      <c r="C6">
+        <v>2738</v>
+      </c>
+      <c r="D6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6">
+        <v>34</v>
+      </c>
+      <c r="F6">
+        <v>11.25</v>
+      </c>
+      <c r="G6">
+        <v>6486</v>
+      </c>
+      <c r="H6">
+        <v>7755.25</v>
+      </c>
+      <c r="I6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7">
+        <v>9000</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7">
+        <v>12</v>
+      </c>
+      <c r="F7">
+        <v>11.25</v>
+      </c>
+      <c r="G7">
+        <v>8988</v>
+      </c>
+      <c r="H7">
+        <v>8999.25</v>
+      </c>
+      <c r="I7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8">
+        <v>10000</v>
+      </c>
+      <c r="C8">
+        <v>2738</v>
+      </c>
+      <c r="D8" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8">
+        <v>3</v>
+      </c>
+      <c r="F8">
+        <v>11.25</v>
+      </c>
+      <c r="G8">
+        <v>8517</v>
+      </c>
+      <c r="H8">
+        <v>9786.25</v>
+      </c>
+      <c r="I8" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9">
+        <v>11000</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <v>11.25</v>
+      </c>
+      <c r="G9">
+        <v>11000</v>
+      </c>
+      <c r="H9">
+        <v>11011.25</v>
+      </c>
+      <c r="I9" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10">
+        <v>12000</v>
+      </c>
+      <c r="C10">
+        <v>2738</v>
+      </c>
+      <c r="D10" t="s">
+        <v>14</v>
+      </c>
+      <c r="E10">
+        <v>26</v>
+      </c>
+      <c r="F10">
+        <v>11.25</v>
+      </c>
+      <c r="G10">
+        <v>10494</v>
+      </c>
+      <c r="H10">
+        <v>11763.25</v>
+      </c>
+      <c r="I10" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11">
+        <v>13000</v>
+      </c>
+      <c r="C11">
+        <v>2738</v>
+      </c>
+      <c r="D11" t="s">
+        <v>16</v>
+      </c>
+      <c r="E11">
+        <v>44</v>
+      </c>
+      <c r="F11">
+        <v>11.25</v>
+      </c>
+      <c r="G11">
+        <v>11476</v>
+      </c>
+      <c r="H11">
+        <v>12745.25</v>
+      </c>
+      <c r="I11" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12">
+        <v>14000</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E12">
+        <v>18</v>
+      </c>
+      <c r="F12">
+        <v>11.25</v>
+      </c>
+      <c r="G12">
+        <v>13982</v>
+      </c>
+      <c r="H12">
+        <v>13993.25</v>
+      </c>
+      <c r="I12" t="s">
+        <v>24</v>
+      </c>
+    </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96FBF4EA-5FD4-4CA3-AADB-8DD58EB52034}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96FBF4EA-5FD4-4CA3-AADB-8DD58EB52034}">
   <dimension ref="A1:J12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K16" sqref="K16"/>
+      <selection activeCell="I12" sqref="A2:I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="14" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="22" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="6" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="9.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="12" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="22" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="16.0" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="11.7109375" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="14.0" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="22.0" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="6.0" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="9.85546875" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="22.0" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="1" s="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -681,11 +914,8 @@
       <c r="I1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="J1" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -713,11 +943,8 @@
       <c r="I2" t="s">
         <v>24</v>
       </c>
-      <c r="J2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -745,11 +972,8 @@
       <c r="I3" t="s">
         <v>24</v>
       </c>
-      <c r="J3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -774,11 +998,8 @@
       <c r="I4" t="s">
         <v>24</v>
       </c>
-      <c r="J4">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -806,11 +1027,8 @@
       <c r="I5" t="s">
         <v>24</v>
       </c>
-      <c r="J5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>15</v>
       </c>
@@ -838,11 +1056,8 @@
       <c r="I6" t="s">
         <v>24</v>
       </c>
-      <c r="J6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>17</v>
       </c>
@@ -870,11 +1085,8 @@
       <c r="I7" t="s">
         <v>24</v>
       </c>
-      <c r="J7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>18</v>
       </c>
@@ -902,11 +1114,8 @@
       <c r="I8" t="s">
         <v>24</v>
       </c>
-      <c r="J8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>19</v>
       </c>
@@ -931,11 +1140,8 @@
       <c r="I9" t="s">
         <v>24</v>
       </c>
-      <c r="J9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>20</v>
       </c>
@@ -963,11 +1169,8 @@
       <c r="I10" t="s">
         <v>24</v>
       </c>
-      <c r="J10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>21</v>
       </c>
@@ -995,11 +1198,8 @@
       <c r="I11" t="s">
         <v>24</v>
       </c>
-      <c r="J11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>22</v>
       </c>
@@ -1027,28 +1227,25 @@
       <c r="I12" t="s">
         <v>24</v>
       </c>
-      <c r="J12">
-        <v>0</v>
-      </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6267371-6AA0-4A44-B06D-B320EDFB1404}">
-  <dimension ref="A1:C2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6267371-6AA0-4A44-B06D-B320EDFB1404}">
+  <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="106" workbookViewId="0">
+    <sheetView workbookViewId="0" zoomScale="106">
       <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.7109375" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="22.5703125" customWidth="1"/>
-    <col min="3" max="3" width="23" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="23.7109375" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="22.5703125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="23.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -1064,17 +1261,17 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B2" t="s">
         <v>12</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup orientation="portrait" paperSize="9" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Adjust test suite for recall and rerun payroll
</commit_message>
<xml_diff>
--- a/Data Files/Test Data.xlsx
+++ b/Data Files/Test Data.xlsx
@@ -1,25 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27932"/>
   <workbookPr defaultThemeVersion="202300"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aditia\git\hre_test\Data Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr documentId="13_ncr:1_{F7D75790-B829-498D-8C7F-686F442780FC}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84ECB15E-01EF-4D89-BAD4-D7E9695AFFCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView windowHeight="15720" windowWidth="29040" xWindow="-120" xr2:uid="{24326381-8BEC-45D3-BC51-8ABD6EF7D704}" yWindow="-120"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{24326381-8BEC-45D3-BC51-8ABD6EF7D704}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" r:id="rId1" sheetId="1"/>
-    <sheet name="Sheet2" r:id="rId2" sheetId="2"/>
-    <sheet name="Test Name" r:id="rId3" sheetId="3"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Test Name" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="30">
   <si>
     <t>Name</t>
   </si>
@@ -113,20 +113,16 @@
     <t>Employee Name</t>
   </si>
   <si>
-    <t>100.00</t>
-  </si>
-  <si>
-    <t>cjaUzEDo</t>
-  </si>
-  <si>
-    <t>MHArryMt</t>
+    <t>rFBOFVYF</t>
+  </si>
+  <si>
+    <t>200.00</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -162,18 +158,18 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" quotePrefix="1" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -190,10 +186,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="0E2841"/>
@@ -228,7 +224,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin panose="02110004020202020204" typeface="Aptos Display"/>
+        <a:latin typeface="Aptos Display" panose="02110004020202020204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -280,7 +276,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin panose="02110004020202020204" typeface="Aptos Narrow"/>
+        <a:latin typeface="Aptos Narrow" panose="02110004020202020204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -391,21 +387,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="25400">
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -422,7 +418,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -494,32 +490,32 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{2E142A2C-CD16-42D6-873A-C26D2A0506FA}" name="Office Theme" vid="{1BDDFF52-6CD6-40A5-AB3C-68EB2F1E4D0A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{2E142A2C-CD16-42D6-873A-C26D2A0506FA}" vid="{1BDDFF52-6CD6-40A5-AB3C-68EB2F1E4D0A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{391E7384-A072-4B6F-A8B1-C9FE83A7EF78}">
-  <dimension ref="A1:J12"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{391E7384-A072-4B6F-A8B1-C9FE83A7EF78}">
+  <dimension ref="A1:I12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A1:I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="16.0" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="11.7109375" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="14.0" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="22.0" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="6.0" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="9.85546875" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
+    <col min="1" max="1" width="16" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="14" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="22" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="6" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="9.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="12" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row customFormat="1" r="1" s="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -862,12 +858,12 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96FBF4EA-5FD4-4CA3-AADB-8DD58EB52034}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96FBF4EA-5FD4-4CA3-AADB-8DD58EB52034}">
   <dimension ref="A1:J12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -876,17 +872,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="16.0" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="11.7109375" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="14.0" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="22.0" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="6.0" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="9.85546875" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="22.0" collapsed="true"/>
+    <col min="1" max="1" width="16" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="14" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="22" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="6" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="9.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="12" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="22" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row customFormat="1" r="1" s="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1229,23 +1225,23 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6267371-6AA0-4A44-B06D-B320EDFB1404}">
-  <dimension ref="A1:D2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6267371-6AA0-4A44-B06D-B320EDFB1404}">
+  <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="106">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView tabSelected="1" zoomScale="106" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="23.7109375" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="22.5703125" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="23.0" collapsed="true"/>
+    <col min="1" max="1" width="23.7109375" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="22.5703125" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="23" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -1261,17 +1257,17 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B2" t="s">
         <v>12</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup orientation="portrait" paperSize="9" r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Enhance create and run payroll single
</commit_message>
<xml_diff>
--- a/Data Files/Test Data.xlsx
+++ b/Data Files/Test Data.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="49">
   <si>
     <t>Name</t>
   </si>
@@ -119,6 +119,60 @@
   </si>
   <si>
     <t>jGyxpyQd</t>
+  </si>
+  <si>
+    <t>kOvIJGxQ</t>
+  </si>
+  <si>
+    <t>wULTFWFe</t>
+  </si>
+  <si>
+    <t>gmFLNnnk</t>
+  </si>
+  <si>
+    <t>bteImEFz</t>
+  </si>
+  <si>
+    <t>pLBnQeiK</t>
+  </si>
+  <si>
+    <t>sQxRkphN</t>
+  </si>
+  <si>
+    <t>JmkYnBbl</t>
+  </si>
+  <si>
+    <t>dyuZgByl</t>
+  </si>
+  <si>
+    <t>gPrVDCsq</t>
+  </si>
+  <si>
+    <t>XLvYUvQA</t>
+  </si>
+  <si>
+    <t>UJiYLLyd</t>
+  </si>
+  <si>
+    <t>yOslshsT</t>
+  </si>
+  <si>
+    <t>IjRhirEs</t>
+  </si>
+  <si>
+    <t>WFKyqXlS</t>
+  </si>
+  <si>
+    <t>yRkZKAym</t>
+  </si>
+  <si>
+    <t>TEJNnjbN</t>
+  </si>
+  <si>
+    <t>KTtpgbMt</t>
+  </si>
+  <si>
+    <t>WjYUAFLI</t>
   </si>
 </sst>
 </file>
@@ -893,7 +947,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>30</v>
+        <v>48</v>
       </c>
       <c r="B2" t="s">
         <v>12</v>

</xml_diff>